<commit_message>
PDF created from selected employees
</commit_message>
<xml_diff>
--- a/src/resources/Place.xlsx
+++ b/src/resources/Place.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Radnici" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -41,13 +41,10 @@
     <t xml:space="preserve">Milković</t>
   </si>
   <si>
-    <t xml:space="preserve">Antonia </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Čančar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mirjana</t>
+    <t xml:space="preserve">Josip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Felix</t>
   </si>
   <si>
     <t xml:space="preserve">Koeficijent</t>
@@ -147,7 +144,76 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
@@ -160,90 +226,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>6000</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -254,11 +237,6 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1.3</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>1.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>